<commit_message>
Complete Application in Scratch Org
</commit_message>
<xml_diff>
--- a/me/4.Working-with-Scratch-Orgs.xlsx
+++ b/me/4.Working-with-Scratch-Orgs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SFDX-and-Salesforce-CLI\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23CA05D-0F33-4477-B939-6822D08C69A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B995A5-0BBF-41CF-AFF3-902CB1971D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Scratch Org" sheetId="1" r:id="rId1"/>
     <sheet name="PushMetadatainScratchOrg" sheetId="3" r:id="rId2"/>
     <sheet name="Upload Data in Scratch Org" sheetId="4" r:id="rId3"/>
+    <sheet name="CompleteApplicationInScratchOrg" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="224">
   <si>
     <t>To create a Scratch Org we need to make sure that we have a Dev Hub Org</t>
   </si>
@@ -852,6 +853,147 @@
   </si>
   <si>
     <t>sfdx force:data:tree:import -p sample-data/import-plan.json</t>
+  </si>
+  <si>
+    <t>sfdx force:lightning:component:create -n newTreePlantation --type lwc -d force-app/main/default/lwc/</t>
+  </si>
+  <si>
+    <t>create new component</t>
+  </si>
+  <si>
+    <t>SFDX-and-Salesforce-CLI\tree-plantation\force-app\main\default\lwc\newTreePlantation\newTreePlantation.html</t>
+  </si>
+  <si>
+    <t>&lt;template&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;lightning-card&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;lightning-button slot="actions" label="Record New Plantation" variant="brand" onclick={recordNewPlantation}&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;/lightning-button&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;template if:true={showForm}&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;lightning-record-form object-api-name="Tree_Plantation__c" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    record-id={recordId} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    layout-type="Full" </t>
+  </si>
+  <si>
+    <t>                    mode={mode}</t>
+  </si>
+  <si>
+    <t>                    onsuccess={handleSuccess}&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;/lightning-record-form&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;/template&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/lightning-card&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/template&gt;</t>
+  </si>
+  <si>
+    <t>just same SFDX-and-Salesforce-CLI\CLISession\force-app\main\default\lwc\newTreePlantation\newTreePlantation.js-meta.xml</t>
+  </si>
+  <si>
+    <t>SFDX-and-Salesforce-CLI\tree-plantation\force-app\main\default\lwc\newTreePlantation\newTreePlantation.js</t>
+  </si>
+  <si>
+    <t>import { LightningElement, track } from 'lwc';</t>
+  </si>
+  <si>
+    <t>import { ShowToastEvent } from 'lightning/platformShowToastEvent';</t>
+  </si>
+  <si>
+    <t>export default class NewTreePlantation extends LightningElement {</t>
+  </si>
+  <si>
+    <t>    @track recordId;</t>
+  </si>
+  <si>
+    <t>    @track showForm = false;</t>
+  </si>
+  <si>
+    <t>    recordNewPlantation(){</t>
+  </si>
+  <si>
+    <t>        this.showForm = true;</t>
+  </si>
+  <si>
+    <t>        this.recordId = undefined;</t>
+  </si>
+  <si>
+    <t>    handleSuccess(event) {</t>
+  </si>
+  <si>
+    <t>        const evt = new ShowToastEvent({</t>
+  </si>
+  <si>
+    <t>            title: "Plantation Recorded",</t>
+  </si>
+  <si>
+    <t>            message: "Record ID: " + event.detail.id,</t>
+  </si>
+  <si>
+    <t>            variant: "success"</t>
+  </si>
+  <si>
+    <t>        });</t>
+  </si>
+  <si>
+    <t>        this.dispatchEvent(evt);</t>
+  </si>
+  <si>
+    <t>    get mode(){</t>
+  </si>
+  <si>
+    <t>        return this.recordId ? 'view' : 'edit';</t>
+  </si>
+  <si>
+    <t>just same SFDX-and-Salesforce-CLI\CLISession\force-app\main\default\lwc\newTreePlantation\newTreePlantation.js</t>
+  </si>
+  <si>
+    <t>SFDX-and-Salesforce-CLI\tree-plantation\force-app\main\default\lwc\treePlantationExplorer\treePlantationExplorer.html</t>
+  </si>
+  <si>
+    <t>    &lt;lightning-tabset&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;lightning-tab label="Tree List" &gt;</t>
+  </si>
+  <si>
+    <t>            &lt;c-tree-list&gt;&lt;/c-tree-list&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;/lightning-tab&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;lightning-tab label="New Plantation"&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;c-new-tree-plantation &gt;&lt;/c-new-tree-plantation&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/lightning-tabset&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run test classes in our Org </t>
+  </si>
+  <si>
+    <t>sfdx force:apex:test:run --testlevel RunAllTestsInOrg --codecoverage --resultformat human</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1165,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3871,6 +4013,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>108239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B62319D3-7FF5-AE1E-A027-9715A0722840}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685801" y="11125200"/>
+          <a:ext cx="11087100" cy="1746539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>347383</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>45142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F8F8B0-AC06-4364-BAA2-03037DDBEB51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="671793" y="24450675"/>
+          <a:ext cx="11172825" cy="4740967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>33399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7F030EF-4086-5823-8DAC-6C6DF3078B56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698046" y="29432250"/>
+          <a:ext cx="11289847" cy="5653149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>104165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A2985AB-068D-4059-85E3-A3F075650753}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695326" y="35909250"/>
+          <a:ext cx="11144250" cy="4390415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -18121,8 +18444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BFD360-A4A5-43A7-B393-D4C85F05A33B}">
   <dimension ref="A3:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18400,7 +18723,7 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="4" t="s">
         <v>147</v>
       </c>
       <c r="L41" s="5"/>
@@ -18462,4 +18785,1153 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F093414-6ACA-4101-BD6D-8D77CA834D02}">
+  <dimension ref="A3:O188"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="G17" t="s">
+        <v>140</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="G30" t="s">
+        <v>136</v>
+      </c>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="G46" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" t="s">
+        <v>142</v>
+      </c>
+      <c r="N46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="H47" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="H48" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="25"/>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="25"/>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="25"/>
+      <c r="D51" t="s">
+        <v>175</v>
+      </c>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="25"/>
+      <c r="D52" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="25"/>
+      <c r="D53" t="s">
+        <v>36</v>
+      </c>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="8"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>179</v>
+      </c>
+      <c r="N69" t="s">
+        <v>142</v>
+      </c>
+      <c r="O69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="3"/>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="5"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="5"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="5"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="5"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="28"/>
+      <c r="K77" s="28"/>
+      <c r="L77" s="28"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="28"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="28"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+      <c r="I82" s="28"/>
+      <c r="J82" s="28"/>
+      <c r="K82" s="28"/>
+      <c r="L82" s="28"/>
+      <c r="M82" s="5"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B83" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>195</v>
+      </c>
+      <c r="M86" t="s">
+        <v>142</v>
+      </c>
+      <c r="N86" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="3"/>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
+      <c r="K88" s="28"/>
+      <c r="L88" s="5"/>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
+      <c r="K89" s="28"/>
+      <c r="L89" s="5"/>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="5"/>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="28"/>
+      <c r="J91" s="28"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="5"/>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="28"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28"/>
+      <c r="I92" s="28"/>
+      <c r="J92" s="28"/>
+      <c r="K92" s="28"/>
+      <c r="L92" s="5"/>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="28"/>
+      <c r="J93" s="28"/>
+      <c r="K93" s="28"/>
+      <c r="L93" s="5"/>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="28"/>
+      <c r="J94" s="28"/>
+      <c r="K94" s="28"/>
+      <c r="L94" s="5"/>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="28"/>
+      <c r="I95" s="28"/>
+      <c r="J95" s="28"/>
+      <c r="K95" s="28"/>
+      <c r="L95" s="5"/>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="28"/>
+      <c r="I96" s="28"/>
+      <c r="J96" s="28"/>
+      <c r="K96" s="28"/>
+      <c r="L96" s="5"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
+      <c r="I97" s="28"/>
+      <c r="J97" s="28"/>
+      <c r="K97" s="28"/>
+      <c r="L97" s="5"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+      <c r="J98" s="28"/>
+      <c r="K98" s="28"/>
+      <c r="L98" s="5"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+      <c r="K99" s="28"/>
+      <c r="L99" s="5"/>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+      <c r="H100" s="28"/>
+      <c r="I100" s="28"/>
+      <c r="J100" s="28"/>
+      <c r="K100" s="28"/>
+      <c r="L100" s="5"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
+      <c r="K101" s="28"/>
+      <c r="L101" s="5"/>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+      <c r="K102" s="28"/>
+      <c r="L102" s="5"/>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="28"/>
+      <c r="J103" s="28"/>
+      <c r="K103" s="28"/>
+      <c r="L103" s="5"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="28"/>
+      <c r="I104" s="28"/>
+      <c r="J104" s="28"/>
+      <c r="K104" s="28"/>
+      <c r="L104" s="5"/>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
+      <c r="I105" s="28"/>
+      <c r="J105" s="28"/>
+      <c r="K105" s="28"/>
+      <c r="L105" s="5"/>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="28"/>
+      <c r="J106" s="28"/>
+      <c r="K106" s="28"/>
+      <c r="L106" s="5"/>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="28"/>
+      <c r="J107" s="28"/>
+      <c r="K107" s="28"/>
+      <c r="L107" s="5"/>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="4"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="28"/>
+      <c r="I108" s="28"/>
+      <c r="J108" s="28"/>
+      <c r="K108" s="28"/>
+      <c r="L108" s="5"/>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="28"/>
+      <c r="I109" s="28"/>
+      <c r="J109" s="28"/>
+      <c r="K109" s="28"/>
+      <c r="L109" s="5"/>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="28"/>
+      <c r="H110" s="28"/>
+      <c r="I110" s="28"/>
+      <c r="J110" s="28"/>
+      <c r="K110" s="28"/>
+      <c r="L110" s="5"/>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="28"/>
+      <c r="K111" s="28"/>
+      <c r="L111" s="5"/>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="8"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="3"/>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="28"/>
+      <c r="G117" s="5"/>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C118" s="28"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="28"/>
+      <c r="F118" s="28"/>
+      <c r="G118" s="5"/>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="5"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C120" s="28"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="28"/>
+      <c r="F120" s="28"/>
+      <c r="G120" s="5"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
+      <c r="G121" s="5"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C122" s="28"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="28"/>
+      <c r="F122" s="28"/>
+      <c r="G122" s="5"/>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C123" s="28"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="28"/>
+      <c r="F123" s="28"/>
+      <c r="G123" s="5"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C124" s="28"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="28"/>
+      <c r="G124" s="5"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="8"/>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>